<commit_message>
Can create gantt chart from order list
</commit_message>
<xml_diff>
--- a/03 - Program Outputs/Chart.xlsx
+++ b/03 - Program Outputs/Chart.xlsx
@@ -24,7 +24,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none">
         <fgColor/>
@@ -37,8 +37,112 @@
         <bgColor/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0EBF5"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF892D2D"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF607023"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2D7C4D"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2A4061"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5D2D69"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF892D2D"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF607023"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -50,8 +154,32 @@
   <cellStyleXfs count="1">
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="0" xfId="0">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="4" fillId="5" fontId="0" numFmtId="0" xfId="0">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="5" fillId="6" fontId="0" numFmtId="0" xfId="0">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="6" fillId="7" fontId="0" numFmtId="0" xfId="0">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="7" fillId="8" fontId="0" numFmtId="0" xfId="0">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="8" fillId="9" fontId="0" numFmtId="0" xfId="0">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="常规" xfId="0"/>
@@ -326,55 +454,208 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" max="702" min="2" style="0" width="3"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="5"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
+      <c r="A1" s="1" t="str">
         <v>M1</v>
       </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2">
-      <c r="A2" t="str">
+      <c r="A2" s="1" t="str">
         <v>M2</v>
       </c>
-      <c r="B2">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="str">
+        <v>M3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="str">
+        <v>M4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="str">
+        <v>M5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="str">
+        <v>M6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="str">
+        <v>M7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="str">
+        <v>M8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="str">
+        <v>M9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="Q10">
+        <v>15</v>
+      </c>
+      <c r="V10">
+        <v>20</v>
+      </c>
+      <c r="AA10">
+        <v>25</v>
+      </c>
+      <c r="AF10">
+        <v>30</v>
+      </c>
+      <c r="AK10">
+        <v>35</v>
+      </c>
+      <c r="AP10">
+        <v>40</v>
+      </c>
+      <c r="AU10">
+        <v>45</v>
+      </c>
+      <c r="AZ10">
+        <v>50</v>
+      </c>
+      <c r="BE10">
+        <v>55</v>
+      </c>
+      <c r="BJ10">
+        <v>60</v>
+      </c>
+      <c r="BO10">
+        <v>65</v>
+      </c>
+      <c r="BT10">
+        <v>70</v>
+      </c>
+      <c r="BY10">
+        <v>75</v>
+      </c>
+      <c r="CD10">
+        <v>80</v>
+      </c>
+      <c r="CI10">
+        <v>85</v>
+      </c>
+      <c r="CN10">
+        <v>90</v>
+      </c>
+      <c r="CS10">
+        <v>95</v>
+      </c>
+      <c r="CX10">
         <v>100</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>M3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>M4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>M5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>M6</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>M7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>M8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>M9</v>
+      <c r="DC10">
+        <v>105</v>
+      </c>
+      <c r="DH10">
+        <v>110</v>
+      </c>
+      <c r="DM10">
+        <v>115</v>
+      </c>
+      <c r="DR10">
+        <v>120</v>
+      </c>
+      <c r="DW10">
+        <v>125</v>
+      </c>
+      <c r="EB10">
+        <v>130</v>
+      </c>
+      <c r="EG10">
+        <v>135</v>
+      </c>
+      <c r="EL10">
+        <v>140</v>
+      </c>
+      <c r="EQ10">
+        <v>145</v>
+      </c>
+      <c r="EV10">
+        <v>150</v>
+      </c>
+      <c r="FA10">
+        <v>155</v>
+      </c>
+      <c r="FF10">
+        <v>160</v>
+      </c>
+      <c r="FK10">
+        <v>165</v>
+      </c>
+      <c r="FP10">
+        <v>170</v>
+      </c>
+      <c r="FU10">
+        <v>175</v>
+      </c>
+      <c r="FZ10">
+        <v>180</v>
+      </c>
+      <c r="GE10">
+        <v>185</v>
+      </c>
+      <c r="GJ10">
+        <v>190</v>
+      </c>
+      <c r="GO10">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="str">
+        <v>Job 0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="str">
+        <v>Job 1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="str">
+        <v>Job 2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="str">
+        <v>Job 3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="str">
+        <v>Job 4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>